<commit_message>
enhance the documentation layout, add more pages to UI section, remove gantt chart file and replace it with the actual table
</commit_message>
<xml_diff>
--- a/Documents/PackTrack-GanttChart.xlsx
+++ b/Documents/PackTrack-GanttChart.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA997E1D-0E4A-46AB-8832-2E9BD8ED8AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\PackTrack\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F3513-FE96-4A7D-840B-9E430DFF240D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -975,16 +980,34 @@
     <xf numFmtId="0" fontId="18" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="14" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -999,26 +1022,8 @@
     <xf numFmtId="166" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2084,7 +2089,7 @@
   <dimension ref="A1:DF35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2124,32 +2129,32 @@
       <c r="E1" s="13"/>
       <c r="F1" s="14"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
       <c r="P1" s="17"/>
-      <c r="Q1" s="94">
+      <c r="Q1" s="100">
         <v>45717</v>
       </c>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93"/>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
     </row>
     <row r="2" spans="1:92" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="83" t="s">
         <v>29</v>
@@ -2157,33 +2162,33 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
       <c r="F2" s="15"/>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="92">
+      <c r="Q2" s="98">
         <v>2</v>
       </c>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="93"/>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="93"/>
-      <c r="Z2" s="93"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
     </row>
     <row r="3" spans="1:92" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="85" t="s">
         <v>13</v>
@@ -2203,142 +2208,142 @@
         <v>13</v>
       </c>
       <c r="E4" s="21"/>
-      <c r="I4" s="97">
+      <c r="I4" s="103">
         <f>I5</f>
         <v>45719</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88">
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97">
         <f>P5</f>
         <v>45726</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97">
         <f>W5</f>
         <v>45733</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="97"/>
+      <c r="Y4" s="97"/>
+      <c r="Z4" s="97"/>
+      <c r="AA4" s="97"/>
+      <c r="AB4" s="97"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="97">
         <f>AD5</f>
         <v>45740</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="97"/>
+      <c r="AF4" s="97"/>
+      <c r="AG4" s="97"/>
+      <c r="AH4" s="97"/>
+      <c r="AI4" s="97"/>
+      <c r="AJ4" s="97"/>
+      <c r="AK4" s="97">
         <f>AK5</f>
         <v>45747</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="97"/>
+      <c r="AM4" s="97"/>
+      <c r="AN4" s="97"/>
+      <c r="AO4" s="97"/>
+      <c r="AP4" s="97"/>
+      <c r="AQ4" s="97"/>
+      <c r="AR4" s="97">
         <f>AR5</f>
         <v>45754</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="97"/>
+      <c r="AT4" s="97"/>
+      <c r="AU4" s="97"/>
+      <c r="AV4" s="97"/>
+      <c r="AW4" s="97"/>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="97">
         <f>AY5</f>
         <v>45761</v>
       </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="97"/>
+      <c r="BB4" s="97"/>
+      <c r="BC4" s="97"/>
+      <c r="BD4" s="97"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="97">
         <f>BF5</f>
         <v>45768</v>
       </c>
-      <c r="BG4" s="88"/>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
-      <c r="BL4" s="89"/>
-      <c r="BM4" s="88">
+      <c r="BG4" s="97"/>
+      <c r="BH4" s="97"/>
+      <c r="BI4" s="97"/>
+      <c r="BJ4" s="97"/>
+      <c r="BK4" s="97"/>
+      <c r="BL4" s="104"/>
+      <c r="BM4" s="97">
         <f>BM5</f>
         <v>45775</v>
       </c>
-      <c r="BN4" s="88"/>
-      <c r="BO4" s="88"/>
-      <c r="BP4" s="88"/>
-      <c r="BQ4" s="88"/>
-      <c r="BR4" s="88"/>
-      <c r="BS4" s="89"/>
-      <c r="BT4" s="88">
+      <c r="BN4" s="97"/>
+      <c r="BO4" s="97"/>
+      <c r="BP4" s="97"/>
+      <c r="BQ4" s="97"/>
+      <c r="BR4" s="97"/>
+      <c r="BS4" s="104"/>
+      <c r="BT4" s="97">
         <f>BT5</f>
         <v>45782</v>
       </c>
-      <c r="BU4" s="88"/>
-      <c r="BV4" s="88"/>
-      <c r="BW4" s="88"/>
-      <c r="BX4" s="88"/>
-      <c r="BY4" s="88"/>
-      <c r="BZ4" s="89"/>
-      <c r="CA4" s="88">
+      <c r="BU4" s="97"/>
+      <c r="BV4" s="97"/>
+      <c r="BW4" s="97"/>
+      <c r="BX4" s="97"/>
+      <c r="BY4" s="97"/>
+      <c r="BZ4" s="104"/>
+      <c r="CA4" s="97">
         <f>CA5</f>
         <v>45789</v>
       </c>
-      <c r="CB4" s="88"/>
-      <c r="CC4" s="88"/>
-      <c r="CD4" s="88"/>
-      <c r="CE4" s="88"/>
-      <c r="CF4" s="88"/>
-      <c r="CG4" s="89"/>
-      <c r="CH4" s="88">
+      <c r="CB4" s="97"/>
+      <c r="CC4" s="97"/>
+      <c r="CD4" s="97"/>
+      <c r="CE4" s="97"/>
+      <c r="CF4" s="97"/>
+      <c r="CG4" s="104"/>
+      <c r="CH4" s="97">
         <f>CH5</f>
         <v>45796</v>
       </c>
-      <c r="CI4" s="88"/>
-      <c r="CJ4" s="88"/>
-      <c r="CK4" s="88"/>
-      <c r="CL4" s="88"/>
-      <c r="CM4" s="88"/>
-      <c r="CN4" s="89"/>
+      <c r="CI4" s="97"/>
+      <c r="CJ4" s="97"/>
+      <c r="CK4" s="97"/>
+      <c r="CL4" s="97"/>
+      <c r="CM4" s="97"/>
+      <c r="CN4" s="104"/>
     </row>
     <row r="5" spans="1:92" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99" t="s">
+      <c r="A5" s="91"/>
+      <c r="B5" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="90" t="s">
+      <c r="D5" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="90" t="s">
+      <c r="E5" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="90" t="s">
+      <c r="F5" s="96" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="22">
@@ -2679,345 +2684,345 @@
       </c>
     </row>
     <row r="6" spans="1:92" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="98"/>
-      <c r="B6" s="100"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="I6" s="102" t="str">
+      <c r="A6" s="91"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="I6" s="88" t="str">
         <f t="shared" ref="I6:AN6" si="19">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="J6" s="103" t="str">
+      <c r="J6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="K6" s="103" t="str">
+      <c r="K6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>W</v>
       </c>
-      <c r="L6" s="103" t="str">
+      <c r="L6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="M6" s="103" t="str">
+      <c r="M6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>F</v>
       </c>
-      <c r="N6" s="103" t="str">
+      <c r="N6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="O6" s="103" t="str">
+      <c r="O6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="P6" s="103" t="str">
+      <c r="P6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>M</v>
       </c>
-      <c r="Q6" s="103" t="str">
+      <c r="Q6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="R6" s="103" t="str">
+      <c r="R6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>W</v>
       </c>
-      <c r="S6" s="103" t="str">
+      <c r="S6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="T6" s="103" t="str">
+      <c r="T6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>F</v>
       </c>
-      <c r="U6" s="103" t="str">
+      <c r="U6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="V6" s="103" t="str">
+      <c r="V6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="W6" s="103" t="str">
+      <c r="W6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>M</v>
       </c>
-      <c r="X6" s="103" t="str">
+      <c r="X6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="Y6" s="103" t="str">
+      <c r="Y6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>W</v>
       </c>
-      <c r="Z6" s="103" t="str">
+      <c r="Z6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="AA6" s="103" t="str">
+      <c r="AA6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>F</v>
       </c>
-      <c r="AB6" s="103" t="str">
+      <c r="AB6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="AC6" s="103" t="str">
+      <c r="AC6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="AD6" s="103" t="str">
+      <c r="AD6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>M</v>
       </c>
-      <c r="AE6" s="103" t="str">
+      <c r="AE6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="AF6" s="103" t="str">
+      <c r="AF6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>W</v>
       </c>
-      <c r="AG6" s="103" t="str">
+      <c r="AG6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="AH6" s="103" t="str">
+      <c r="AH6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>F</v>
       </c>
-      <c r="AI6" s="103" t="str">
+      <c r="AI6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="AJ6" s="103" t="str">
+      <c r="AJ6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>S</v>
       </c>
-      <c r="AK6" s="103" t="str">
+      <c r="AK6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>M</v>
       </c>
-      <c r="AL6" s="103" t="str">
+      <c r="AL6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="AM6" s="103" t="str">
+      <c r="AM6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>W</v>
       </c>
-      <c r="AN6" s="103" t="str">
+      <c r="AN6" s="89" t="str">
         <f t="shared" si="19"/>
         <v>T</v>
       </c>
-      <c r="AO6" s="103" t="str">
+      <c r="AO6" s="89" t="str">
         <f t="shared" ref="AO6:BL6" si="20">LEFT(TEXT(AO5,"ddd"),1)</f>
         <v>F</v>
       </c>
-      <c r="AP6" s="103" t="str">
+      <c r="AP6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="AQ6" s="103" t="str">
+      <c r="AQ6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="AR6" s="103" t="str">
+      <c r="AR6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>M</v>
       </c>
-      <c r="AS6" s="103" t="str">
+      <c r="AS6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>T</v>
       </c>
-      <c r="AT6" s="103" t="str">
+      <c r="AT6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>W</v>
       </c>
-      <c r="AU6" s="103" t="str">
+      <c r="AU6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>T</v>
       </c>
-      <c r="AV6" s="103" t="str">
+      <c r="AV6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>F</v>
       </c>
-      <c r="AW6" s="103" t="str">
+      <c r="AW6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="AX6" s="103" t="str">
+      <c r="AX6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="AY6" s="103" t="str">
+      <c r="AY6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>M</v>
       </c>
-      <c r="AZ6" s="103" t="str">
+      <c r="AZ6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>T</v>
       </c>
-      <c r="BA6" s="103" t="str">
+      <c r="BA6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>W</v>
       </c>
-      <c r="BB6" s="103" t="str">
+      <c r="BB6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>T</v>
       </c>
-      <c r="BC6" s="103" t="str">
+      <c r="BC6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>F</v>
       </c>
-      <c r="BD6" s="103" t="str">
+      <c r="BD6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="BE6" s="103" t="str">
+      <c r="BE6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="BF6" s="103" t="str">
+      <c r="BF6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>M</v>
       </c>
-      <c r="BG6" s="103" t="str">
+      <c r="BG6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>T</v>
       </c>
-      <c r="BH6" s="103" t="str">
+      <c r="BH6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>W</v>
       </c>
-      <c r="BI6" s="103" t="str">
+      <c r="BI6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>T</v>
       </c>
-      <c r="BJ6" s="103" t="str">
+      <c r="BJ6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>F</v>
       </c>
-      <c r="BK6" s="103" t="str">
+      <c r="BK6" s="89" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="BL6" s="104" t="str">
+      <c r="BL6" s="90" t="str">
         <f t="shared" si="20"/>
         <v>S</v>
       </c>
-      <c r="BM6" s="103" t="str">
+      <c r="BM6" s="89" t="str">
         <f t="shared" ref="BM6:BS6" si="21">LEFT(TEXT(BM5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="BN6" s="103" t="str">
+      <c r="BN6" s="89" t="str">
         <f t="shared" si="21"/>
         <v>T</v>
       </c>
-      <c r="BO6" s="103" t="str">
+      <c r="BO6" s="89" t="str">
         <f t="shared" si="21"/>
         <v>W</v>
       </c>
-      <c r="BP6" s="103" t="str">
+      <c r="BP6" s="89" t="str">
         <f t="shared" si="21"/>
         <v>T</v>
       </c>
-      <c r="BQ6" s="103" t="str">
+      <c r="BQ6" s="89" t="str">
         <f t="shared" si="21"/>
         <v>F</v>
       </c>
-      <c r="BR6" s="103" t="str">
+      <c r="BR6" s="89" t="str">
         <f t="shared" si="21"/>
         <v>S</v>
       </c>
-      <c r="BS6" s="104" t="str">
+      <c r="BS6" s="90" t="str">
         <f t="shared" si="21"/>
         <v>S</v>
       </c>
-      <c r="BT6" s="103" t="str">
+      <c r="BT6" s="89" t="str">
         <f t="shared" ref="BT6:CN6" si="22">LEFT(TEXT(BT5,"ddd"),1)</f>
         <v>M</v>
       </c>
-      <c r="BU6" s="103" t="str">
+      <c r="BU6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="BV6" s="103" t="str">
+      <c r="BV6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>W</v>
       </c>
-      <c r="BW6" s="103" t="str">
+      <c r="BW6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="BX6" s="103" t="str">
+      <c r="BX6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>F</v>
       </c>
-      <c r="BY6" s="103" t="str">
+      <c r="BY6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>S</v>
       </c>
-      <c r="BZ6" s="104" t="str">
+      <c r="BZ6" s="90" t="str">
         <f t="shared" si="22"/>
         <v>S</v>
       </c>
-      <c r="CA6" s="103" t="str">
+      <c r="CA6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>M</v>
       </c>
-      <c r="CB6" s="103" t="str">
+      <c r="CB6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="CC6" s="103" t="str">
+      <c r="CC6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>W</v>
       </c>
-      <c r="CD6" s="103" t="str">
+      <c r="CD6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="CE6" s="103" t="str">
+      <c r="CE6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>F</v>
       </c>
-      <c r="CF6" s="103" t="str">
+      <c r="CF6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>S</v>
       </c>
-      <c r="CG6" s="104" t="str">
+      <c r="CG6" s="90" t="str">
         <f t="shared" si="22"/>
         <v>S</v>
       </c>
-      <c r="CH6" s="103" t="str">
+      <c r="CH6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>M</v>
       </c>
-      <c r="CI6" s="103" t="str">
+      <c r="CI6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="CJ6" s="103" t="str">
+      <c r="CJ6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>W</v>
       </c>
-      <c r="CK6" s="103" t="str">
+      <c r="CK6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>T</v>
       </c>
-      <c r="CL6" s="103" t="str">
+      <c r="CL6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>F</v>
       </c>
-      <c r="CM6" s="103" t="str">
+      <c r="CM6" s="89" t="str">
         <f t="shared" si="22"/>
         <v>S</v>
       </c>
-      <c r="CN6" s="104" t="str">
+      <c r="CN6" s="90" t="str">
         <f t="shared" si="22"/>
         <v>S</v>
       </c>
@@ -5246,11 +5251,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="F5:F6"/>
@@ -5263,11 +5268,11 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D28">
     <cfRule type="dataBar" priority="88">
@@ -5550,6 +5555,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5861,36 +5895,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5911,33 +5943,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>